<commit_message>
Completion of Report Formatting Extensions!
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/ModelReport/ModelReportTemplate.xlsx
+++ b/Src/SummitReports.Objects/Reports/ModelReport/ModelReportTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Summit\SummitReports\Src\SummitReports.Objects\Reports\ModelReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68B8AB7-A0C0-4647-B040-CA59950913A5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5341FEF-0B31-48D2-934B-CFB251A65785}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BidPoolData" sheetId="8" state="hidden" r:id="rId1"/>
@@ -1382,9 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8448AB60-5AB7-48FE-BAAA-2DC17B57AC99}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Added alignment and examples of cloning sheets
</commit_message>
<xml_diff>
--- a/Src/SummitReports.Objects/Reports/ModelReport/ModelReportTemplate.xlsx
+++ b/Src/SummitReports.Objects/Reports/ModelReport/ModelReportTemplate.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Summit\SummitReports\Src\SummitReports.Objects\Reports\ModelReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5341FEF-0B31-48D2-934B-CFB251A65785}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5035006D-83D2-4EB1-90AE-D6A5D0E48615}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BidPoolData" sheetId="8" state="hidden" r:id="rId1"/>
     <sheet name="RelationshipData" sheetId="9" state="hidden" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId3"/>
+    <sheet name="MODEL" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" iterateDelta="1E-4"/>
   <extLst>
@@ -1382,7 +1382,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8448AB60-5AB7-48FE-BAAA-2DC17B57AC99}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>